<commit_message>
Actualización lista de materiales
</commit_message>
<xml_diff>
--- a/Lista_materiales.xlsx
+++ b/Lista_materiales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegofigueroa/Documents/GitHub/bibliotecas_autoprestamo_UNAL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Documents\GitHub\bibliotecas_autoprestamo_UNAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C6D355-857D-CB47-8F6A-6E8506407830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA129330-BEF9-4CF9-8B38-F2CC5A9C2EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{6EFF0760-D250-D548-B1D7-DC577D3B340D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6EFF0760-D250-D548-B1D7-DC577D3B340D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -984,22 +984,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3CD313-03E6-244B-AE88-DF23578FE24D}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1025,12 +1025,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -1051,12 +1051,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>13</v>
@@ -1077,12 +1077,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
@@ -1103,7 +1103,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>149</v>
       </c>
@@ -1129,12 +1129,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>23</v>
@@ -1155,7 +1155,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -1286,12 +1286,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>38</v>
@@ -1312,7 +1312,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
@@ -1338,12 +1338,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>68</v>
@@ -1364,12 +1364,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>51</v>
@@ -1390,7 +1390,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>53</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>140</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>67</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>71</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>132</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>77</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>133</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>82</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>84</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>86</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>89</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>92</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>96</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>100</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>31</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>106</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>109</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>135</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>136</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>119</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>123</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>126</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>129</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>34</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>141</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>138</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>151</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>

</xml_diff>